<commit_message>
Added draft for 3rd paper
</commit_message>
<xml_diff>
--- a/proposal_assignments.xlsx
+++ b/proposal_assignments.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\workspaces_local\cs598_dl4hc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E00DD0E-630A-4F83-8F7D-C05CD958D84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="1524" yWindow="-96" windowWidth="21612" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +88,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,13 +131,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -131,6 +155,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -179,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,9 +239,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,21 +483,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
@@ -447,69 +508,69 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>2.1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="1">
         <v>2.4</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="1">
         <v>2.5</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1">
         <v>2.6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1">
         <v>2.7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -520,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -531,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1">
         <v>3.1</v>
       </c>
@@ -539,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1">
         <v>3.1</v>
       </c>
@@ -547,7 +608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="1">
         <v>3.1</v>
       </c>
@@ -555,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="1">
         <v>3.1</v>
       </c>
@@ -563,7 +624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1">
         <v>3.1</v>
       </c>
@@ -571,65 +632,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -640,24 +701,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>